<commit_message>
update main layout and logic
</commit_message>
<xml_diff>
--- a/av.xlsx
+++ b/av.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\INKALI-PC\project\INKALI_QC_DX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69C79DD9-5CAD-455D-9DB4-54F3F6F85CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E98EC3-3513-4C9A-AE03-7928D68D7F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{AF3DB4E7-CB92-45F5-80E7-460D1B758F36}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
   <si>
     <t>lot</t>
   </si>
@@ -73,6 +73,24 @@
   </si>
   <si>
     <t>percobaan ke-</t>
+  </si>
+  <si>
+    <t>A130302P</t>
+  </si>
+  <si>
+    <t>PACKING</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>AZHAR</t>
+  </si>
+  <si>
+    <t>DAFIQ</t>
   </si>
 </sst>
 </file>
@@ -108,13 +126,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -125,6 +148,29 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0B56AF66-380D-4F44-9216-1FCFB25D2EC5}" name="Table1" displayName="Table1" ref="A1:L7" totalsRowShown="0">
+  <autoFilter ref="A1:L7" xr:uid="{0B56AF66-380D-4F44-9216-1FCFB25D2EC5}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{0E05E104-5D7C-48A0-AB42-83A8F7640FC0}" name="lot"/>
+    <tableColumn id="2" xr3:uid="{7AB95A7A-9ED0-4A3B-A6AD-88A75F380A84}" name="percobaan ke-"/>
+    <tableColumn id="3" xr3:uid="{E95F329E-9D57-46B8-90C8-2F8079880DB1}" name="waktu"/>
+    <tableColumn id="4" xr3:uid="{1EABB9DA-A669-48F7-A0BC-8056817C0283}" name="temperatur"/>
+    <tableColumn id="5" xr3:uid="{700246D3-E204-4727-A0BD-C61AE1A02C2A}" name="berat sampel (gr)"/>
+    <tableColumn id="6" xr3:uid="{C0D53F63-3F55-4AB6-815B-7BCD12EA2F66}" name="jumlah titran (mL)"/>
+    <tableColumn id="7" xr3:uid="{6DD57BB5-6560-41D8-88F3-DBC89BA73D51}" name="faktor buret"/>
+    <tableColumn id="8" xr3:uid="{A7BB2AB5-6A9B-445C-8292-B9AEAD388D0B}" name="faktor NaOH"/>
+    <tableColumn id="9" xr3:uid="{BA92A53D-9895-404E-9034-3DDE49D4E948}" name="acid value" dataDxfId="0">
+      <calculatedColumnFormula>(Table1[[#This Row],[jumlah titran (mL)]]*Table1[[#This Row],[faktor buret]]*Table1[[#This Row],[faktor NaOH]]*5.61)/Table1[[#This Row],[berat sampel (gr)]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{49929249-B88F-443F-B28D-011432691767}" name="keputusan"/>
+    <tableColumn id="11" xr3:uid="{231F0FE0-F528-4B2B-AC31-160D2617BFAA}" name="operator QA"/>
+    <tableColumn id="12" xr3:uid="{481393E5-2AD6-4768-A8C5-BCEF7C8F7728}" name="operator produksi"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -424,23 +470,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB1827DE-B1D3-42C1-AF55-F93FF216D822}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.36328125" customWidth="1"/>
-    <col min="4" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" customWidth="1"/>
+    <col min="3" max="3" width="7.90625" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="17.08984375" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" customWidth="1"/>
+    <col min="7" max="7" width="12.81640625" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" customWidth="1"/>
+    <col min="9" max="9" width="11.08984375" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" customWidth="1"/>
+    <col min="11" max="11" width="13.1796875" customWidth="1"/>
+    <col min="12" max="12" width="17.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
@@ -481,8 +529,245 @@
         <v>10</v>
       </c>
     </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D2">
+        <v>70</v>
+      </c>
+      <c r="E2">
+        <v>0.40279999999999999</v>
+      </c>
+      <c r="F2">
+        <v>6.984</v>
+      </c>
+      <c r="G2">
+        <v>1.0044999999999999</v>
+      </c>
+      <c r="H2">
+        <v>1.0025999999999999</v>
+      </c>
+      <c r="I2">
+        <f>(Table1[[#This Row],[jumlah titran (mL)]]*Table1[[#This Row],[faktor buret]]*Table1[[#This Row],[faktor NaOH]]*5.61)/Table1[[#This Row],[berat sampel (gr)]]</f>
+        <v>97.961465026832158</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D3">
+        <v>180</v>
+      </c>
+      <c r="E3">
+        <v>1.0765</v>
+      </c>
+      <c r="F3">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="G3">
+        <v>1.0044999999999999</v>
+      </c>
+      <c r="H3">
+        <v>1.0025999999999999</v>
+      </c>
+      <c r="I3">
+        <f>(Table1[[#This Row],[jumlah titran (mL)]]*Table1[[#This Row],[faktor buret]]*Table1[[#This Row],[faktor NaOH]]*5.61)/Table1[[#This Row],[berat sampel (gr)]]</f>
+        <v>24.824905799359037</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D4">
+        <v>225</v>
+      </c>
+      <c r="E4">
+        <v>1.2110000000000001</v>
+      </c>
+      <c r="F4">
+        <v>3.2789999999999999</v>
+      </c>
+      <c r="G4">
+        <v>1.0044999999999999</v>
+      </c>
+      <c r="H4">
+        <v>1.0025999999999999</v>
+      </c>
+      <c r="I4">
+        <f>(Table1[[#This Row],[jumlah titran (mL)]]*Table1[[#This Row],[faktor buret]]*Table1[[#This Row],[faktor NaOH]]*5.61)/Table1[[#This Row],[berat sampel (gr)]]</f>
+        <v>15.298109886641615</v>
+      </c>
+      <c r="J4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D5">
+        <v>225</v>
+      </c>
+      <c r="E5">
+        <v>2.0735999999999999</v>
+      </c>
+      <c r="F5">
+        <v>2.927</v>
+      </c>
+      <c r="G5">
+        <v>1.0044999999999999</v>
+      </c>
+      <c r="H5">
+        <v>1.0025999999999999</v>
+      </c>
+      <c r="I5">
+        <f>(Table1[[#This Row],[jumlah titran (mL)]]*Table1[[#This Row],[faktor buret]]*Table1[[#This Row],[faktor NaOH]]*5.61)/Table1[[#This Row],[berat sampel (gr)]]</f>
+        <v>7.9751386267838544</v>
+      </c>
+      <c r="J5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.59375</v>
+      </c>
+      <c r="D6">
+        <v>225</v>
+      </c>
+      <c r="E6">
+        <v>3.0247999999999999</v>
+      </c>
+      <c r="F6">
+        <v>3.7290000000000001</v>
+      </c>
+      <c r="G6">
+        <v>1.0044999999999999</v>
+      </c>
+      <c r="H6">
+        <v>1.0025999999999999</v>
+      </c>
+      <c r="I6">
+        <f>(Table1[[#This Row],[jumlah titran (mL)]]*Table1[[#This Row],[faktor buret]]*Table1[[#This Row],[faktor NaOH]]*5.61)/Table1[[#This Row],[berat sampel (gr)]]</f>
+        <v>6.965242184399961</v>
+      </c>
+      <c r="J6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>3.3450000000000002</v>
+      </c>
+      <c r="F7">
+        <v>3.569</v>
+      </c>
+      <c r="G7">
+        <v>1.0044999999999999</v>
+      </c>
+      <c r="H7">
+        <v>1.0025999999999999</v>
+      </c>
+      <c r="I7">
+        <f>(Table1[[#This Row],[jumlah titran (mL)]]*Table1[[#This Row],[faktor buret]]*Table1[[#This Row],[faktor NaOH]]*5.61)/Table1[[#This Row],[berat sampel (gr)]]</f>
+        <v>6.0282454700905825</v>
+      </c>
+      <c r="J7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -499,15 +784,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x01010090999A988820A941B81692230FA37518" ma:contentTypeVersion="8" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="82af067276d17f8da8878e59c9fc26dd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fa79aa9a-415f-460d-87f7-8f1f5ec238dc" xmlns:ns4="df19daa0-827c-44d1-82f8-b684d8942059" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d9231dfc705bd5ed2140636435699610" ns3:_="" ns4:_="">
     <xsd:import namespace="fa79aa9a-415f-460d-87f7-8f1f5ec238dc"/>
@@ -698,6 +974,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -707,14 +992,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71B7F3D9-9ACE-4A5A-A88D-437E59AB8860}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{032A24FC-289D-47E3-BC57-7F457615F887}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -733,6 +1010,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71B7F3D9-9ACE-4A5A-A88D-437E59AB8860}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35AE4DEE-966C-4FE9-917D-8A5BFAD0D03E}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
add handling errors on input
</commit_message>
<xml_diff>
--- a/av.xlsx
+++ b/av.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\INKALI-PC\project\INKALI_QC_DX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC7F3AD-5C45-4027-A125-B0DADECF230B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58B2633-F3FF-40E5-A2C8-708AE9A5D686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{AF3DB4E7-CB92-45F5-80E7-460D1B758F36}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{AF3DB4E7-CB92-45F5-80E7-460D1B758F36}"/>
   </bookViews>
   <sheets>
     <sheet name="ACID VALUE" sheetId="1" r:id="rId1"/>
-    <sheet name="HF SERIES" sheetId="2" r:id="rId2"/>
+    <sheet name="s1200" sheetId="3" r:id="rId2"/>
+    <sheet name="HF SERIES" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
   <si>
     <t>lot</t>
   </si>
@@ -91,6 +92,36 @@
   </si>
   <si>
     <t>DAFIQ</t>
+  </si>
+  <si>
+    <t>LOT</t>
+  </si>
+  <si>
+    <t>Suhu</t>
+  </si>
+  <si>
+    <t>Berat Sample (gr)</t>
+  </si>
+  <si>
+    <t>Jumlah Titran (mL)</t>
+  </si>
+  <si>
+    <t>Faktor Buret</t>
+  </si>
+  <si>
+    <t>Faktor NaOH</t>
+  </si>
+  <si>
+    <t>AV</t>
+  </si>
+  <si>
+    <t>Instruksi</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Operator QC</t>
   </si>
 </sst>
 </file>
@@ -472,7 +503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB1827DE-B1D3-42C1-AF55-F93FF216D822}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
@@ -772,6 +803,61 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{817FFF9F-43E0-49A3-9A8C-74DBE47261BD}">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.90625" customWidth="1"/>
+    <col min="10" max="10" width="11.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ED30A4F-DF17-4B85-B827-66EDC4724F55}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -784,23 +870,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fa79aa9a-415f-460d-87f7-8f1f5ec238dc" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x01010090999A988820A941B81692230FA37518" ma:contentTypeVersion="8" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="82af067276d17f8da8878e59c9fc26dd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fa79aa9a-415f-460d-87f7-8f1f5ec238dc" xmlns:ns4="df19daa0-827c-44d1-82f8-b684d8942059" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d9231dfc705bd5ed2140636435699610" ns3:_="" ns4:_="">
     <xsd:import namespace="fa79aa9a-415f-460d-87f7-8f1f5ec238dc"/>
@@ -991,32 +1060,24 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fa79aa9a-415f-460d-87f7-8f1f5ec238dc" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35AE4DEE-966C-4FE9-917D-8A5BFAD0D03E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="df19daa0-827c-44d1-82f8-b684d8942059"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="fa79aa9a-415f-460d-87f7-8f1f5ec238dc"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71B7F3D9-9ACE-4A5A-A88D-437E59AB8860}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{032A24FC-289D-47E3-BC57-7F457615F887}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1033,4 +1094,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71B7F3D9-9ACE-4A5A-A88D-437E59AB8860}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35AE4DEE-966C-4FE9-917D-8A5BFAD0D03E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="df19daa0-827c-44d1-82f8-b684d8942059"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="fa79aa9a-415f-460d-87f7-8f1f5ec238dc"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add logic to instruksi
</commit_message>
<xml_diff>
--- a/av.xlsx
+++ b/av.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -573,10 +573,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+      <c r="A4" t="n">
+        <v>12</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -586,10 +584,8 @@
           <t>13:53</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
+      <c r="D4" t="n">
+        <v>21</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -614,6 +610,534 @@
       <c r="K4" t="inlineStr">
         <is>
           <t>testing purposes</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>12</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>10:18</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>12</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Packing</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>12</v>
+      </c>
+      <c r="G5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H5" t="n">
+        <v>12</v>
+      </c>
+      <c r="I5" t="n">
+        <v>12</v>
+      </c>
+      <c r="J5" t="n">
+        <v>9694.08</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>testing purposes</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>12</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>10:18</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>12</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Packing</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>12</v>
+      </c>
+      <c r="G6" t="n">
+        <v>12</v>
+      </c>
+      <c r="H6" t="n">
+        <v>12</v>
+      </c>
+      <c r="I6" t="n">
+        <v>12</v>
+      </c>
+      <c r="J6" t="n">
+        <v>9694.08</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>testing purposes</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>12</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>10:19</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>12</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Packing</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>12</v>
+      </c>
+      <c r="G7" t="n">
+        <v>12</v>
+      </c>
+      <c r="H7" t="n">
+        <v>12345</v>
+      </c>
+      <c r="I7" t="n">
+        <v>12</v>
+      </c>
+      <c r="J7" t="n">
+        <v>10259502363</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>testing purposes</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>A1234P</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>10:22</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>faris</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Packing</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" t="n">
+        <v>5.61</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>testing purposes</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>A12212P</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>10:58</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>FARIS</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>10</v>
+      </c>
+      <c r="G9" t="n">
+        <v>5</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="n">
+        <v>2.805</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>lakukan pemanasan hingga 240°C</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>A12212P</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>10:59</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>FARIS</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>10</v>
+      </c>
+      <c r="G10" t="n">
+        <v>5</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" t="n">
+        <v>2.805</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Lakukan cooling hingga 120°C</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>A12212P</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>10:59</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>FARIS</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>10</v>
+      </c>
+      <c r="G11" t="n">
+        <v>50</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" t="n">
+        <v>28.05</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Tambah waktu pemanasan</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>A12212P</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>10:59</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>FARIS</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>10</v>
+      </c>
+      <c r="G12" t="n">
+        <v>50</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" t="n">
+        <v>28.05</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Hubungi atasan</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>A12212P</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>5</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>10:59</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>FARIS</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>10</v>
+      </c>
+      <c r="G13" t="n">
+        <v>5</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" t="n">
+        <v>2.805</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Tambah Oleic Acid</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>1212</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>11:20</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>12</v>
+      </c>
+      <c r="G14" t="n">
+        <v>12</v>
+      </c>
+      <c r="H14" t="n">
+        <v>12</v>
+      </c>
+      <c r="I14" t="n">
+        <v>12</v>
+      </c>
+      <c r="J14" t="n">
+        <v>9694.08</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>lakukan pemanasan hingga 240°C</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>12</v>
+      </c>
+      <c r="G15" t="n">
+        <v>12</v>
+      </c>
+      <c r="H15" t="n">
+        <v>12</v>
+      </c>
+      <c r="I15" t="n">
+        <v>12</v>
+      </c>
+      <c r="J15" t="n">
+        <v>9694.08</v>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>lakukan pemanasan hingga 240°C</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Packing</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>12</v>
+      </c>
+      <c r="G16" t="n">
+        <v>12</v>
+      </c>
+      <c r="H16" t="n">
+        <v>12</v>
+      </c>
+      <c r="I16" t="n">
+        <v>12</v>
+      </c>
+      <c r="J16" t="n">
+        <v>9694.08</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>NG</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
create form for AV PEG 600DO-IK optimize from S1200-IK form with simple library package "openpyxl" rather than "pandas"
</commit_message>
<xml_diff>
--- a/av.xlsx
+++ b/av.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1141,6 +1141,96 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>4123</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>14:32</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>12</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" t="n">
+        <v>12</v>
+      </c>
+      <c r="I17" t="n">
+        <v>12</v>
+      </c>
+      <c r="J17" t="n">
+        <v>807.84</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Hubungi atasan</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>14:35</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>12</v>
+      </c>
+      <c r="G18" t="n">
+        <v>12</v>
+      </c>
+      <c r="H18" t="n">
+        <v>12</v>
+      </c>
+      <c r="I18" t="n">
+        <v>12</v>
+      </c>
+      <c r="J18" t="n">
+        <v>9694.08</v>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Hubungi atasan</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>